<commit_message>
Reading to buffer is no longer blocked, returns event instead
</commit_message>
<xml_diff>
--- a/OpenCL_SMA/Testing_Strategy/Milestone1/Performance Comparison.xlsx
+++ b/OpenCL_SMA/Testing_Strategy/Milestone1/Performance Comparison.xlsx
@@ -223,9 +223,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -234,6 +231,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -553,7 +553,7 @@
   <dimension ref="J7:S13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,55 +563,55 @@
   </cols>
   <sheetData>
     <row r="7" spans="10:19" x14ac:dyDescent="0.25">
-      <c r="J7" s="18"/>
-      <c r="K7" s="13" t="s">
+      <c r="J7" s="17"/>
+      <c r="K7" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13" t="s">
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13" t="s">
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
     </row>
     <row r="8" spans="10:19" x14ac:dyDescent="0.25">
-      <c r="J8" s="19"/>
-      <c r="K8" s="14" t="s">
+      <c r="J8" s="18"/>
+      <c r="K8" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="L8" s="14" t="s">
+      <c r="L8" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="M8" s="14" t="s">
+      <c r="M8" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="N8" s="14" t="s">
+      <c r="N8" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="O8" s="14" t="s">
+      <c r="O8" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="P8" s="14" t="s">
+      <c r="P8" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="Q8" s="14" t="s">
+      <c r="Q8" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="R8" s="14" t="s">
+      <c r="R8" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="S8" s="14" t="s">
+      <c r="S8" s="13" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="10:19" x14ac:dyDescent="0.25">
-      <c r="J9" s="15">
+      <c r="J9" s="14">
         <v>100</v>
       </c>
       <c r="K9" s="1">
@@ -632,7 +632,7 @@
       <c r="S9" s="3"/>
     </row>
     <row r="10" spans="10:19" x14ac:dyDescent="0.25">
-      <c r="J10" s="16">
+      <c r="J10" s="15">
         <v>1000</v>
       </c>
       <c r="K10" s="4">
@@ -653,7 +653,7 @@
       <c r="S10" s="6"/>
     </row>
     <row r="11" spans="10:19" x14ac:dyDescent="0.25">
-      <c r="J11" s="16">
+      <c r="J11" s="15">
         <v>10000</v>
       </c>
       <c r="K11" s="4">
@@ -674,7 +674,7 @@
       <c r="S11" s="6"/>
     </row>
     <row r="12" spans="10:19" x14ac:dyDescent="0.25">
-      <c r="J12" s="16">
+      <c r="J12" s="15">
         <v>100000</v>
       </c>
       <c r="K12" s="4">
@@ -695,18 +695,18 @@
       <c r="S12" s="6"/>
     </row>
     <row r="13" spans="10:19" x14ac:dyDescent="0.25">
-      <c r="J13" s="17">
+      <c r="J13" s="16">
         <v>1000000</v>
       </c>
       <c r="K13" s="7">
-        <v>6483</v>
+        <v>5485</v>
       </c>
       <c r="L13" s="8">
         <v>10155</v>
       </c>
       <c r="M13" s="12">
         <f t="shared" si="0"/>
-        <v>1.5664044423877834</v>
+        <v>1.8514129443938012</v>
       </c>
       <c r="N13" s="8"/>
       <c r="O13" s="8"/>

</xml_diff>

<commit_message>
updates to performance analysis
</commit_message>
<xml_diff>
--- a/OpenCL_SMA/Testing_Strategy/Milestone1/Performance Comparison.xlsx
+++ b/OpenCL_SMA/Testing_Strategy/Milestone1/Performance Comparison.xlsx
@@ -48,13 +48,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -209,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -235,6 +241,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -550,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="J7:S13"/>
+  <dimension ref="J7:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,14 +624,14 @@
         <v>100</v>
       </c>
       <c r="K9" s="1">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="L9" s="2">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="M9" s="10">
         <f>L9/K9</f>
-        <v>1.5</v>
+        <v>2.3636363636363638</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -636,14 +645,14 @@
         <v>1000</v>
       </c>
       <c r="K10" s="4">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="L10" s="5">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="M10" s="11">
         <f>L10/K10</f>
-        <v>1.05</v>
+        <v>1.4705882352941178</v>
       </c>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
@@ -657,14 +666,14 @@
         <v>10000</v>
       </c>
       <c r="K11" s="4">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="L11" s="5">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="M11" s="11">
         <f t="shared" ref="M11:M13" si="0">L11/K11</f>
-        <v>0.89075630252100846</v>
+        <v>1.4186046511627908</v>
       </c>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
@@ -678,14 +687,14 @@
         <v>100000</v>
       </c>
       <c r="K12" s="4">
-        <v>681</v>
+        <v>623</v>
       </c>
       <c r="L12" s="5">
-        <v>917</v>
+        <v>966</v>
       </c>
       <c r="M12" s="11">
         <f t="shared" si="0"/>
-        <v>1.3465491923641704</v>
+        <v>1.550561797752809</v>
       </c>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
@@ -699,14 +708,14 @@
         <v>1000000</v>
       </c>
       <c r="K13" s="7">
-        <v>5485</v>
+        <v>5725</v>
       </c>
       <c r="L13" s="8">
-        <v>10155</v>
+        <v>12097</v>
       </c>
       <c r="M13" s="12">
         <f t="shared" si="0"/>
-        <v>1.8514129443938012</v>
+        <v>2.1130131004366812</v>
       </c>
       <c r="N13" s="8"/>
       <c r="O13" s="8"/>
@@ -714,6 +723,9 @@
       <c r="Q13" s="8"/>
       <c r="R13" s="8"/>
       <c r="S13" s="9"/>
+    </row>
+    <row r="19" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L19" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
first draft with OpenCL new line parser
</commit_message>
<xml_diff>
--- a/OpenCL_SMA/Testing_Strategy/Milestone1/Performance Comparison.xlsx
+++ b/OpenCL_SMA/Testing_Strategy/Milestone1/Performance Comparison.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VirturalRealityGreenspace\OpenCL_SMA\Testing_Strategy\Milestone1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\GreenSpaceVirtualReality\OpenCL_SMA\Testing_Strategy\Milestone1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18915" windowHeight="13500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -215,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -233,6 +233,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -241,9 +251,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -559,180 +566,262 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="J7:S19"/>
+  <dimension ref="J7:V24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="16" max="16" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="10:19" x14ac:dyDescent="0.25">
-      <c r="J7" s="17"/>
-      <c r="K7" s="19" t="s">
+    <row r="7" spans="10:22" x14ac:dyDescent="0.25">
+      <c r="J7" s="23"/>
+      <c r="K7" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19" t="s">
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="O7" s="19"/>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="19" t="s">
+      <c r="Q7" s="25"/>
+      <c r="R7" s="25"/>
+      <c r="S7" s="25"/>
+      <c r="T7" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="R7" s="19"/>
-      <c r="S7" s="19"/>
+      <c r="U7" s="25"/>
+      <c r="V7" s="25"/>
     </row>
-    <row r="8" spans="10:19" x14ac:dyDescent="0.25">
-      <c r="J8" s="18"/>
+    <row r="8" spans="10:22" x14ac:dyDescent="0.25">
+      <c r="J8" s="24"/>
       <c r="K8" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="L8" s="13" t="s">
+      <c r="L8" s="13"/>
+      <c r="M8" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="M8" s="13" t="s">
+      <c r="N8" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="N8" s="13" t="s">
+      <c r="O8" s="13"/>
+      <c r="P8" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="O8" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="P8" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q8" s="13" t="s">
-        <v>1</v>
-      </c>
+      <c r="Q8" s="13"/>
       <c r="R8" s="13" t="s">
         <v>0</v>
       </c>
       <c r="S8" s="13" t="s">
         <v>5</v>
       </c>
+      <c r="T8" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="U8" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="V8" s="13" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="9" spans="10:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="10:22" x14ac:dyDescent="0.25">
       <c r="J9" s="14">
         <v>100</v>
       </c>
       <c r="K9" s="1">
         <v>11</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L9" s="2"/>
+      <c r="M9" s="2">
         <v>26</v>
       </c>
-      <c r="M9" s="10">
-        <f>L9/K9</f>
+      <c r="N9" s="10">
+        <f>M9/K9</f>
         <v>2.3636363636363638</v>
       </c>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="3"/>
+      <c r="O9" s="20">
+        <v>14</v>
+      </c>
+      <c r="P9" s="2">
+        <v>16</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>4</v>
+      </c>
+      <c r="R9" s="2">
+        <v>15</v>
+      </c>
+      <c r="S9" s="10">
+        <f>R9/P9</f>
+        <v>0.9375</v>
+      </c>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="3"/>
     </row>
-    <row r="10" spans="10:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="10:22" x14ac:dyDescent="0.25">
       <c r="J10" s="15">
         <v>1000</v>
       </c>
       <c r="K10" s="4">
         <v>17</v>
       </c>
-      <c r="L10" s="5">
+      <c r="L10" s="5"/>
+      <c r="M10" s="5">
         <v>25</v>
       </c>
-      <c r="M10" s="11">
-        <f>L10/K10</f>
+      <c r="N10" s="11">
+        <f>M10/K10</f>
         <v>1.4705882352941178</v>
       </c>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="6"/>
+      <c r="O10" s="21">
+        <v>11</v>
+      </c>
+      <c r="P10" s="19">
+        <v>19</v>
+      </c>
+      <c r="Q10" s="19">
+        <v>4</v>
+      </c>
+      <c r="R10" s="19">
+        <v>20</v>
+      </c>
+      <c r="S10" s="11">
+        <f>R10/P10</f>
+        <v>1.0526315789473684</v>
+      </c>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="6"/>
     </row>
-    <row r="11" spans="10:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="10:22" x14ac:dyDescent="0.25">
       <c r="J11" s="15">
         <v>10000</v>
       </c>
       <c r="K11" s="4">
         <v>86</v>
       </c>
-      <c r="L11" s="5">
+      <c r="L11" s="5"/>
+      <c r="M11" s="5">
         <v>122</v>
       </c>
-      <c r="M11" s="11">
-        <f t="shared" ref="M11:M13" si="0">L11/K11</f>
+      <c r="N11" s="11">
+        <f t="shared" ref="N11:N13" si="0">M11/K11</f>
         <v>1.4186046511627908</v>
       </c>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="6"/>
+      <c r="O11" s="21">
+        <v>53</v>
+      </c>
+      <c r="P11" s="19">
+        <v>56</v>
+      </c>
+      <c r="Q11" s="19">
+        <v>17</v>
+      </c>
+      <c r="R11" s="19">
+        <v>77</v>
+      </c>
+      <c r="S11" s="11">
+        <f t="shared" ref="S11:S13" si="1">R11/P11</f>
+        <v>1.375</v>
+      </c>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="6"/>
     </row>
-    <row r="12" spans="10:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="10:22" x14ac:dyDescent="0.25">
       <c r="J12" s="15">
         <v>100000</v>
       </c>
       <c r="K12" s="4">
         <v>623</v>
       </c>
-      <c r="L12" s="5">
+      <c r="L12" s="5"/>
+      <c r="M12" s="5">
         <v>966</v>
       </c>
-      <c r="M12" s="11">
+      <c r="N12" s="11">
         <f t="shared" si="0"/>
         <v>1.550561797752809</v>
       </c>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="6"/>
+      <c r="O12" s="21">
+        <v>476</v>
+      </c>
+      <c r="P12" s="19">
+        <v>491</v>
+      </c>
+      <c r="Q12" s="19">
+        <v>165</v>
+      </c>
+      <c r="R12" s="19">
+        <v>836</v>
+      </c>
+      <c r="S12" s="11">
+        <f t="shared" si="1"/>
+        <v>1.7026476578411405</v>
+      </c>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="6"/>
     </row>
-    <row r="13" spans="10:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="10:22" x14ac:dyDescent="0.25">
       <c r="J13" s="16">
         <v>1000000</v>
       </c>
       <c r="K13" s="7">
         <v>5725</v>
       </c>
-      <c r="L13" s="8">
+      <c r="L13" s="8"/>
+      <c r="M13" s="8">
         <v>12097</v>
       </c>
-      <c r="M13" s="12">
+      <c r="N13" s="12">
         <f t="shared" si="0"/>
         <v>2.1130131004366812</v>
       </c>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="9"/>
+      <c r="O13" s="22">
+        <v>46270</v>
+      </c>
+      <c r="P13" s="8">
+        <v>4716</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>1714</v>
+      </c>
+      <c r="R13" s="8">
+        <v>8074</v>
+      </c>
+      <c r="S13" s="12">
+        <f t="shared" si="1"/>
+        <v>1.7120441051738762</v>
+      </c>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="9"/>
     </row>
-    <row r="19" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L19" s="20"/>
+    <row r="19" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="M19" s="17"/>
+    </row>
+    <row r="24" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K24">
+        <f>150*10000</f>
+        <v>1500000</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="P7:S7"/>
+    <mergeCell ref="T7:V7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
added comments and file summary info.  Small optimizations to reduce processing time.
</commit_message>
<xml_diff>
--- a/OpenCL_SMA/Testing_Strategy/Milestone1/Performance Comparison.xlsx
+++ b/OpenCL_SMA/Testing_Strategy/Milestone1/Performance Comparison.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>R</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>Speedup</t>
+  </si>
+  <si>
+    <t>OpenCL</t>
   </si>
 </sst>
 </file>
@@ -566,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="J7:W35"/>
+  <dimension ref="J7:X35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="V19" sqref="V19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,7 +724,7 @@
         <v>53</v>
       </c>
       <c r="P11" s="19">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="Q11" s="19">
         <v>17</v>
@@ -731,7 +734,7 @@
       </c>
       <c r="S11" s="11">
         <f t="shared" ref="S11:S13" si="1">R11/P11</f>
-        <v>3.347826086956522</v>
+        <v>6.416666666666667</v>
       </c>
       <c r="T11" s="5"/>
       <c r="U11" s="5"/>
@@ -756,7 +759,7 @@
         <v>476</v>
       </c>
       <c r="P12" s="19">
-        <v>127</v>
+        <v>82</v>
       </c>
       <c r="Q12" s="19">
         <v>165</v>
@@ -766,7 +769,7 @@
       </c>
       <c r="S12" s="11">
         <f t="shared" si="1"/>
-        <v>6.5826771653543306</v>
+        <v>10.195121951219512</v>
       </c>
       <c r="T12" s="5"/>
       <c r="U12" s="5"/>
@@ -791,7 +794,7 @@
         <v>46270</v>
       </c>
       <c r="P13" s="8">
-        <v>1180</v>
+        <v>711</v>
       </c>
       <c r="Q13" s="8">
         <v>1714</v>
@@ -801,144 +804,125 @@
       </c>
       <c r="S13" s="12">
         <f t="shared" si="1"/>
-        <v>6.8423728813559324</v>
+        <v>11.355836849507735</v>
       </c>
       <c r="T13" s="8"/>
       <c r="U13" s="8"/>
       <c r="V13" s="9"/>
     </row>
-    <row r="19" spans="11:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="11:24" x14ac:dyDescent="0.25">
+      <c r="P18" t="s">
+        <v>6</v>
+      </c>
+      <c r="V18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="11:24" x14ac:dyDescent="0.25">
       <c r="M19" s="17"/>
-      <c r="N19">
-        <v>154</v>
-      </c>
       <c r="P19">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="20" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="N20">
-        <f>296-157</f>
-        <v>139</v>
-      </c>
-      <c r="O20">
-        <f>N19+N20</f>
-        <v>293</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="Q19">
+        <v>12</v>
+      </c>
+      <c r="R19">
+        <v>12</v>
+      </c>
+      <c r="V19">
+        <v>14</v>
+      </c>
+      <c r="W19">
+        <v>15</v>
+      </c>
+      <c r="X19">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="11:24" x14ac:dyDescent="0.25">
       <c r="P20">
-        <v>296</v>
+        <v>13</v>
       </c>
       <c r="Q20">
-        <f>P20-P19</f>
-        <v>139</v>
-      </c>
-    </row>
-    <row r="21" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="N21">
-        <v>140</v>
-      </c>
-      <c r="O21">
-        <f>293+140</f>
-        <v>433</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="R20">
+        <v>12</v>
+      </c>
+      <c r="V20">
+        <v>17</v>
+      </c>
+      <c r="W20">
+        <v>20</v>
+      </c>
+      <c r="X20">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="11:24" x14ac:dyDescent="0.25">
       <c r="P21">
-        <v>436</v>
+        <v>12</v>
       </c>
       <c r="Q21">
-        <f t="shared" ref="Q21:Q27" si="2">P21-P20</f>
-        <v>140</v>
+        <v>15</v>
+      </c>
+      <c r="R21">
+        <v>15</v>
+      </c>
+      <c r="V21">
+        <v>77</v>
       </c>
       <c r="W21">
-        <f>15867000</f>
-        <v>15867000</v>
-      </c>
-    </row>
-    <row r="22" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="N22">
-        <v>115</v>
-      </c>
-      <c r="O22">
-        <f>O21+115</f>
-        <v>548</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="X21">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="11:24" x14ac:dyDescent="0.25">
       <c r="P22">
-        <v>551</v>
+        <v>82</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="2"/>
-        <v>115</v>
+        <v>81</v>
+      </c>
+      <c r="R22">
+        <v>81</v>
+      </c>
+      <c r="V22">
+        <v>836</v>
       </c>
       <c r="W22">
-        <f>W21/150</f>
-        <v>105780</v>
-      </c>
-    </row>
-    <row r="23" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="N23">
-        <v>102</v>
-      </c>
-      <c r="O23">
-        <f>N23+O22</f>
-        <v>650</v>
-      </c>
+        <v>869</v>
+      </c>
+      <c r="X22">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="23" spans="11:24" x14ac:dyDescent="0.25">
       <c r="P23">
-        <v>658</v>
+        <v>711</v>
       </c>
       <c r="Q23">
-        <f t="shared" si="2"/>
-        <v>107</v>
-      </c>
-    </row>
-    <row r="24" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="N24">
-        <v>97</v>
-      </c>
-      <c r="P24">
-        <v>814</v>
-      </c>
-      <c r="Q24">
-        <f t="shared" si="2"/>
-        <v>156</v>
-      </c>
-    </row>
-    <row r="25" spans="11:23" x14ac:dyDescent="0.25">
+        <v>716</v>
+      </c>
+      <c r="R23">
+        <v>711</v>
+      </c>
+      <c r="V23">
+        <v>8074</v>
+      </c>
+      <c r="W23">
+        <v>8259</v>
+      </c>
+      <c r="X23">
+        <v>7755</v>
+      </c>
+    </row>
+    <row r="25" spans="11:24" x14ac:dyDescent="0.25">
       <c r="K25">
         <f>10000/250</f>
         <v>40</v>
-      </c>
-      <c r="N25">
-        <v>162</v>
-      </c>
-      <c r="P25">
-        <v>969</v>
-      </c>
-      <c r="Q25">
-        <f t="shared" si="2"/>
-        <v>155</v>
-      </c>
-    </row>
-    <row r="26" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="N26">
-        <v>150</v>
-      </c>
-      <c r="P26">
-        <v>1096</v>
-      </c>
-      <c r="Q26">
-        <f t="shared" si="2"/>
-        <v>127</v>
-      </c>
-    </row>
-    <row r="27" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="N27">
-        <v>127</v>
-      </c>
-      <c r="P27">
-        <v>1288</v>
-      </c>
-      <c r="Q27">
-        <f t="shared" si="2"/>
-        <v>192</v>
       </c>
     </row>
     <row r="34" spans="10:10" x14ac:dyDescent="0.25">

</xml_diff>